<commit_message>
Final fix for W1.
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Wavelength-Dashboard.xlsx
+++ b/blueprint-jira-better-excel/Wavelength-Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FD8F25-0A9F-4CF4-B499-562B3CC4595D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9912612-C09F-4FF6-9080-2FBA6B375F28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="189" r:id="rId19"/>
+    <pivotCache cacheId="255" r:id="rId19"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -4748,6 +4748,24 @@
                 <c:pt idx="1">
                   <c:v>200</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8085,6 +8103,24 @@
                 <c:pt idx="1">
                   <c:v>200</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10232,6 +10268,24 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
@@ -21596,21 +21650,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
+                <c15:showLeaderLines val="0"/>
               </c:ext>
             </c:extLst>
           </c:dLbls>
@@ -21653,6 +21693,24 @@
                   <c:v>470</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>470</c:v>
                 </c:pt>
               </c:numCache>
@@ -43501,7 +43559,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43886.778058796299" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="109" xr:uid="{00000000-000A-0000-FFFF-FFFF0C000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43886.875072800925" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="109" xr:uid="{00000000-000A-0000-FFFF-FFFF0C000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -49308,8 +49366,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000002000000}" name="PivotTable2" cacheId="189" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
-  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable3" cacheId="255" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A40:A41" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -49338,7 +49396,7 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49376,9 +49434,146 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="45" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable1" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="AB5:AD10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item x="1"/>
+        <item m="1" x="11"/>
+        <item m="1" x="7"/>
+        <item m="1" x="13"/>
+        <item m="1" x="15"/>
+        <item m="1" x="10"/>
+        <item m="1" x="6"/>
+        <item m="1" x="14"/>
+        <item m="1" x="12"/>
+        <item m="1" x="5"/>
+        <item m="1" x="16"/>
+        <item m="1" x="8"/>
+        <item m="1" x="18"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="11">
+        <item h="1" x="0"/>
+        <item m="1" x="8"/>
+        <item m="1" x="9"/>
+        <item h="1" x="1"/>
+        <item m="1" x="6"/>
+        <item m="1" x="7"/>
+        <item h="1" m="1" x="4"/>
+        <item h="1" m="1" x="5"/>
+        <item h="1" x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
@@ -49392,187 +49587,49 @@
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="-2"/>
+    <field x="10"/>
   </rowFields>
   <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
     <i>
       <x/>
     </i>
     <i i="1">
       <x v="1"/>
     </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
   </colItems>
   <pageFields count="3">
-    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="32" hier="-1"/>
     <pageField fld="1" hier="-1"/>
     <pageField fld="45" item="1" hier="-1"/>
   </pageFields>
-  <dataFields count="5">
-    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
-    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
-    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
-    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
-    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  <dataFields count="2">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="10" baseItem="0"/>
+    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="10" baseItem="0"/>
   </dataFields>
-  <chartFormats count="15">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -49585,8 +49642,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000007000000}" name="PivotTable9" cacheId="189" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000007000000}" name="PivotTable9" cacheId="255" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
   <location ref="G29:H34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49995,352 +50052,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31FCE1EF-625E-43F6-9928-8FD8FD0AC1EA}" name="PivotTable11" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="E51:F60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="10">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="3"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="44"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Story Points" fld="13" baseField="44" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="18">
-    <chartFormat chart="2" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="16">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="17">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="18">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable1" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable1" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="AL10:AP17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -50512,7 +50225,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D8B9FB5-5471-4500-848C-1623DA7CC3A0}" name="PivotTable4" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D8B9FB5-5471-4500-848C-1623DA7CC3A0}" name="PivotTable4" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G5:H8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField showAll="0"/>
@@ -50636,7 +50349,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable5" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable5" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -50742,7 +50455,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000000000000}" name="PivotTable1" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000000000000}" name="PivotTable1" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
   <location ref="A6:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -50986,7 +50699,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0A00-000000000000}" name="PivotTable1" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0A00-000000000000}" name="PivotTable1" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B5:C13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -51263,7 +50976,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0C00-000000000000}" name="PivotTable2" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0C00-000000000000}" name="PivotTable2" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D5:E13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -51588,7 +51301,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000000000000}" name="PivotTable1" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000000000000}" name="PivotTable1" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="B9:C15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -52014,7 +51727,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000002000000}" name="PivotTable3" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000002000000}" name="PivotTable3" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="B29:H38" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -52411,178 +52124,127 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000004000000}" name="PivotTable4" cacheId="189" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
-  <location ref="D29:E34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31FCE1EF-625E-43F6-9928-8FD8FD0AC1EA}" name="PivotTable11" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="E51:F60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item m="1" x="7"/>
-        <item x="1"/>
-        <item m="1" x="13"/>
-        <item m="1" x="15"/>
-        <item m="1" x="10"/>
-        <item m="1" x="6"/>
-        <item m="1" x="14"/>
-        <item m="1" x="12"/>
-        <item m="1" x="5"/>
-        <item m="1" x="16"/>
-        <item m="1" x="8"/>
-        <item m="1" x="18"/>
-        <item x="2"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="8"/>
-        <item m="1" x="9"/>
-        <item x="1"/>
-        <item m="1" x="6"/>
-        <item m="1" x="7"/>
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
+      <items count="9">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="7"/>
         <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
         <item x="1"/>
-        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="-2"/>
+    <field x="44"/>
   </rowFields>
-  <rowItems count="5">
+  <rowItems count="9">
     <i>
-      <x/>
-    </i>
-    <i i="1">
       <x v="1"/>
     </i>
-    <i i="2">
+    <i>
       <x v="2"/>
     </i>
-    <i i="3">
+    <i>
       <x v="3"/>
     </i>
-    <i i="4">
+    <i>
       <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
     </i>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
-  <pageFields count="4">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="14" hier="-1"/>
-    <pageField fld="45" item="1" hier="-1"/>
+  <pageFields count="1">
+    <pageField fld="1" item="2" hier="-1"/>
   </pageFields>
-  <dataFields count="5">
-    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
-    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
-    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
-    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
-    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  <dataFields count="1">
+    <dataField name="Sum of Story Points" fld="13" baseField="44" baseItem="0"/>
   </dataFields>
-  <chartFormats count="21">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
+  <chartFormats count="18">
+    <chartFormat chart="2" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -52591,16 +52253,103 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
+    <chartFormat chart="2" format="2">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
             <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="11">
+    <chartFormat chart="2" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="10" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -52609,146 +52358,98 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="12">
+    <chartFormat chart="3" format="11">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
             <x v="1"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="13">
+    <chartFormat chart="3" format="12">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
             <x v="2"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="14">
+    <chartFormat chart="3" format="13">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
             <x v="4"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="15">
+    <chartFormat chart="3" format="15">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="5"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="4" format="22" series="1">
+    <chartFormat chart="3" format="16">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="6"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="4" format="23">
+    <chartFormat chart="3" format="17">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="7"/>
           </reference>
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="4" format="24">
+    <chartFormat chart="3" format="18">
       <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
+        <references count="2">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
           </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="21">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
+          <reference field="44" count="1" selected="0">
+            <x v="8"/>
           </reference>
         </references>
       </pivotArea>
@@ -52767,413 +52468,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000006000000}" name="PivotTable8" cacheId="189" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="G41:G42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item m="1" x="7"/>
-        <item x="1"/>
-        <item m="1" x="13"/>
-        <item m="1" x="15"/>
-        <item m="1" x="10"/>
-        <item m="1" x="6"/>
-        <item m="1" x="14"/>
-        <item m="1" x="12"/>
-        <item m="1" x="5"/>
-        <item m="1" x="16"/>
-        <item m="1" x="8"/>
-        <item m="1" x="18"/>
-        <item x="2"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="8"/>
-        <item m="1" x="9"/>
-        <item x="1"/>
-        <item m="1" x="6"/>
-        <item m="1" x="7"/>
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="17" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable1" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="AB5:AD10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item x="1"/>
-        <item m="1" x="11"/>
-        <item m="1" x="7"/>
-        <item m="1" x="13"/>
-        <item m="1" x="15"/>
-        <item m="1" x="10"/>
-        <item m="1" x="6"/>
-        <item m="1" x="14"/>
-        <item m="1" x="12"/>
-        <item m="1" x="5"/>
-        <item m="1" x="16"/>
-        <item m="1" x="8"/>
-        <item m="1" x="18"/>
-        <item x="2"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="11">
-        <item h="1" x="0"/>
-        <item m="1" x="8"/>
-        <item m="1" x="9"/>
-        <item h="1" x="1"/>
-        <item m="1" x="6"/>
-        <item m="1" x="7"/>
-        <item h="1" m="1" x="4"/>
-        <item h="1" m="1" x="5"/>
-        <item h="1" x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="10"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="45" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="10" baseItem="0"/>
-    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="10" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable3" cacheId="189" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A40:A41" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="8"/>
-        <item m="1" x="9"/>
-        <item x="1"/>
-        <item m="1" x="6"/>
-        <item m="1" x="7"/>
-        <item m="1" x="4"/>
-        <item m="1" x="5"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="45" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFE64A30-B41F-4AE4-94E0-976FA0DF52E6}" name="PivotTable6" cacheId="189" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFE64A30-B41F-4AE4-94E0-976FA0DF52E6}" name="PivotTable6" cacheId="255" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
   <location ref="J29:K34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -53636,8 +52931,642 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FEE7328-E767-497A-8049-35A88773E794}" name="PivotTable7" cacheId="189" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000002000000}" name="PivotTable2" cacheId="255" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="8"/>
+        <item m="1" x="9"/>
+        <item x="1"/>
+        <item m="1" x="6"/>
+        <item m="1" x="7"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="45" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
+    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
+    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
+    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
+    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  </dataFields>
+  <chartFormats count="15">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000004000000}" name="PivotTable4" cacheId="255" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
+  <location ref="D29:E34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item m="1" x="7"/>
+        <item x="1"/>
+        <item m="1" x="13"/>
+        <item m="1" x="15"/>
+        <item m="1" x="10"/>
+        <item m="1" x="6"/>
+        <item m="1" x="14"/>
+        <item m="1" x="12"/>
+        <item m="1" x="5"/>
+        <item m="1" x="16"/>
+        <item m="1" x="8"/>
+        <item m="1" x="18"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="8"/>
+        <item m="1" x="9"/>
+        <item x="1"/>
+        <item m="1" x="6"/>
+        <item m="1" x="7"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="4">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="14" hier="-1"/>
+    <pageField fld="45" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
+    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
+    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
+    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
+    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  </dataFields>
+  <chartFormats count="21">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FEE7328-E767-497A-8049-35A88773E794}" name="PivotTable7" cacheId="255" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="J41:J42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -53765,8 +53694,137 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000006000000}" name="PivotTable8" cacheId="255" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="G41:G42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item m="1" x="7"/>
+        <item x="1"/>
+        <item m="1" x="13"/>
+        <item m="1" x="15"/>
+        <item m="1" x="10"/>
+        <item m="1" x="6"/>
+        <item m="1" x="14"/>
+        <item m="1" x="12"/>
+        <item m="1" x="5"/>
+        <item m="1" x="16"/>
+        <item m="1" x="8"/>
+        <item m="1" x="18"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="8"/>
+        <item m="1" x="9"/>
+        <item x="1"/>
+        <item m="1" x="6"/>
+        <item m="1" x="7"/>
+        <item m="1" x="4"/>
+        <item m="1" x="5"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="17" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable10" cacheId="189" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable10" cacheId="255" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A54:B60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -53932,7 +53990,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000005000000}" name="PivotTable5" cacheId="189" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000005000000}" name="PivotTable5" cacheId="255" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D41:D42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -60700,7 +60758,7 @@
     <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1"/>
@@ -62780,7 +62838,10 @@
         <v>43900</v>
       </c>
       <c r="D5" s="57"/>
-      <c r="E5" s="58"/>
+      <c r="E5" s="58">
+        <f>_ReleaseData!$Q$25</f>
+        <v>470</v>
+      </c>
       <c r="F5" s="40"/>
       <c r="G5" s="40"/>
       <c r="H5" s="40"/>
@@ -62794,7 +62855,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L5" s="59"/>
-      <c r="M5" s="58"/>
+      <c r="M5" s="58">
+        <f>_ReleaseData!$Q$26</f>
+        <v>200</v>
+      </c>
       <c r="N5" s="40"/>
       <c r="O5" s="40"/>
       <c r="P5" s="40"/>
@@ -62808,7 +62872,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="T5" s="57"/>
-      <c r="U5" s="58"/>
+      <c r="U5" s="58">
+        <f>_ReleaseData!$Q$27</f>
+        <v>200</v>
+      </c>
       <c r="V5" s="40"/>
       <c r="W5" s="40"/>
       <c r="X5" s="40"/>
@@ -62822,7 +62889,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AB5" s="57"/>
-      <c r="AC5" s="58"/>
+      <c r="AC5" s="58">
+        <f>_ReleaseData!$Q$28</f>
+        <v>60</v>
+      </c>
       <c r="AD5" s="40"/>
       <c r="AE5" s="40"/>
       <c r="AF5" s="40"/>
@@ -62847,7 +62917,10 @@
         <v>43914</v>
       </c>
       <c r="D6" s="57"/>
-      <c r="E6" s="58"/>
+      <c r="E6" s="58">
+        <f>_ReleaseData!$Q$25</f>
+        <v>470</v>
+      </c>
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
@@ -62861,7 +62934,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L6" s="59"/>
-      <c r="M6" s="58"/>
+      <c r="M6" s="58">
+        <f>_ReleaseData!$Q$26</f>
+        <v>200</v>
+      </c>
       <c r="N6" s="40"/>
       <c r="O6" s="40"/>
       <c r="P6" s="40"/>
@@ -62875,7 +62951,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="T6" s="57"/>
-      <c r="U6" s="58"/>
+      <c r="U6" s="58">
+        <f>_ReleaseData!$Q$27</f>
+        <v>200</v>
+      </c>
       <c r="V6" s="40"/>
       <c r="W6" s="40"/>
       <c r="X6" s="40"/>
@@ -62889,7 +62968,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AB6" s="57"/>
-      <c r="AC6" s="58"/>
+      <c r="AC6" s="58">
+        <f>_ReleaseData!$Q$28</f>
+        <v>60</v>
+      </c>
       <c r="AD6" s="40"/>
       <c r="AE6" s="40"/>
       <c r="AF6" s="40"/>
@@ -62914,7 +62996,10 @@
         <v>43928</v>
       </c>
       <c r="D7" s="57"/>
-      <c r="E7" s="58"/>
+      <c r="E7" s="58">
+        <f>_ReleaseData!$Q$25</f>
+        <v>470</v>
+      </c>
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
       <c r="H7" s="40"/>
@@ -62928,7 +63013,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L7" s="59"/>
-      <c r="M7" s="58"/>
+      <c r="M7" s="58">
+        <f>_ReleaseData!$Q$26</f>
+        <v>200</v>
+      </c>
       <c r="N7" s="40"/>
       <c r="O7" s="40"/>
       <c r="P7" s="40"/>
@@ -62942,7 +63030,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="T7" s="57"/>
-      <c r="U7" s="58"/>
+      <c r="U7" s="58">
+        <f>_ReleaseData!$Q$27</f>
+        <v>200</v>
+      </c>
       <c r="V7" s="40"/>
       <c r="W7" s="40"/>
       <c r="X7" s="40"/>
@@ -62956,7 +63047,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AB7" s="57"/>
-      <c r="AC7" s="58"/>
+      <c r="AC7" s="58">
+        <f>_ReleaseData!$Q$28</f>
+        <v>60</v>
+      </c>
       <c r="AD7" s="40"/>
       <c r="AE7" s="40"/>
       <c r="AF7" s="40"/>
@@ -62987,7 +63081,10 @@
         <v>43942</v>
       </c>
       <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
+      <c r="E8" s="58">
+        <f>_ReleaseData!$Q$25</f>
+        <v>470</v>
+      </c>
       <c r="F8" s="40"/>
       <c r="G8" s="40"/>
       <c r="H8" s="40"/>
@@ -63001,7 +63098,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L8" s="59"/>
-      <c r="M8" s="58"/>
+      <c r="M8" s="58">
+        <f>_ReleaseData!$Q$26</f>
+        <v>200</v>
+      </c>
       <c r="N8" s="40"/>
       <c r="O8" s="40"/>
       <c r="P8" s="40"/>
@@ -63015,7 +63115,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="T8" s="57"/>
-      <c r="U8" s="58"/>
+      <c r="U8" s="58">
+        <f>_ReleaseData!$Q$27</f>
+        <v>200</v>
+      </c>
       <c r="V8" s="40"/>
       <c r="W8" s="40"/>
       <c r="X8" s="40"/>
@@ -63029,7 +63132,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AB8" s="57"/>
-      <c r="AC8" s="58"/>
+      <c r="AC8" s="58">
+        <f>_ReleaseData!$Q$28</f>
+        <v>60</v>
+      </c>
       <c r="AD8" s="40"/>
       <c r="AE8" s="40"/>
       <c r="AF8" s="40"/>
@@ -63060,7 +63166,10 @@
         <v>43956</v>
       </c>
       <c r="D9" s="57"/>
-      <c r="E9" s="58"/>
+      <c r="E9" s="58">
+        <f>_ReleaseData!$Q$25</f>
+        <v>470</v>
+      </c>
       <c r="F9" s="40"/>
       <c r="G9" s="40"/>
       <c r="H9" s="40"/>
@@ -63074,7 +63183,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L9" s="59"/>
-      <c r="M9" s="58"/>
+      <c r="M9" s="58">
+        <f>_ReleaseData!$Q$26</f>
+        <v>200</v>
+      </c>
       <c r="N9" s="40"/>
       <c r="O9" s="40"/>
       <c r="P9" s="40"/>
@@ -63088,7 +63200,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="T9" s="57"/>
-      <c r="U9" s="58"/>
+      <c r="U9" s="58">
+        <f>_ReleaseData!$Q$27</f>
+        <v>200</v>
+      </c>
       <c r="V9" s="40"/>
       <c r="W9" s="40"/>
       <c r="X9" s="40"/>
@@ -63102,7 +63217,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AB9" s="57"/>
-      <c r="AC9" s="58"/>
+      <c r="AC9" s="58">
+        <f>_ReleaseData!$Q$28</f>
+        <v>60</v>
+      </c>
       <c r="AD9" s="40"/>
       <c r="AE9" s="40"/>
       <c r="AF9" s="40"/>
@@ -63127,7 +63245,10 @@
         <v>43970</v>
       </c>
       <c r="D10" s="57"/>
-      <c r="E10" s="58"/>
+      <c r="E10" s="58">
+        <f>_ReleaseData!$Q$25</f>
+        <v>470</v>
+      </c>
       <c r="F10" s="40"/>
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
@@ -63141,7 +63262,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="L10" s="59"/>
-      <c r="M10" s="58"/>
+      <c r="M10" s="58">
+        <f>_ReleaseData!$Q$26</f>
+        <v>200</v>
+      </c>
       <c r="N10" s="40"/>
       <c r="O10" s="40"/>
       <c r="P10" s="40"/>
@@ -63155,7 +63279,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="T10" s="57"/>
-      <c r="U10" s="58"/>
+      <c r="U10" s="58">
+        <f>_ReleaseData!$Q$27</f>
+        <v>200</v>
+      </c>
       <c r="V10" s="40"/>
       <c r="W10" s="40"/>
       <c r="X10" s="40"/>
@@ -63169,7 +63296,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="AB10" s="57"/>
-      <c r="AC10" s="58"/>
+      <c r="AC10" s="58">
+        <f>_ReleaseData!$Q$28</f>
+        <v>60</v>
+      </c>
       <c r="AD10" s="40"/>
       <c r="AE10" s="40"/>
       <c r="AF10" s="40"/>

</xml_diff>

<commit_message>
Adjusted the target scopes of Release and Admin by 60 SP (what is done in Venus).
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Wavelength-Dashboard.xlsx
+++ b/blueprint-jira-better-excel/Wavelength-Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88364F3-D71B-460E-BD59-EB5152920A3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4261542C-476A-4AD8-8BEA-F0ABC4D4A32D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="46" r:id="rId19"/>
+    <pivotCache cacheId="30" r:id="rId19"/>
   </pivotCaches>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -3816,25 +3816,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>173.13432835820896</c:v>
+                  <c:v>225.07462686567166</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>143.28358208955225</c:v>
+                  <c:v>186.26865671641792</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>113.43283582089553</c:v>
+                  <c:v>147.46268656716421</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>83.582089552238799</c:v>
+                  <c:v>108.65671641791045</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>56.716417910447767</c:v>
+                  <c:v>73.731343283582106</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>26.865671641791057</c:v>
+                  <c:v>34.925373134328375</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -4761,28 +4761,28 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>200</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>200</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>200</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>200</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>200</c:v>
+                  <c:v>260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -20813,25 +20813,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>470</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>406.8656716417911</c:v>
+                  <c:v>458.80597014925377</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>336.71641791044777</c:v>
+                  <c:v>379.70149253731347</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>266.56716417910451</c:v>
+                  <c:v>300.59701492537317</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>196.41791044776119</c:v>
+                  <c:v>221.49253731343282</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>133.28358208955225</c:v>
+                  <c:v>150.29850746268659</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>63.134328358208982</c:v>
+                  <c:v>71.194029850746304</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -21765,28 +21765,28 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>470</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>470</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>470</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>470</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>470</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>470</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>470</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>470</c:v>
+                  <c:v>530</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -43634,7 +43634,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43887.324144675928" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="109" xr:uid="{00000000-000A-0000-FFFF-FFFF0C000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43887.4569849537" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="109" xr:uid="{00000000-000A-0000-FFFF-FFFF0C000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -49441,8 +49441,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000004000000}" name="PivotTable4" cacheId="46" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
-  <location ref="D29:E34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000005000000}" name="PivotTable5" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="D41:D42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -49494,7 +49494,7 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49532,258 +49532,31 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
+  <rowItems count="1">
+    <i/>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
-  <pageFields count="4">
+  <pageFields count="3">
     <pageField fld="32" item="9" hier="-1"/>
     <pageField fld="1" hier="-1"/>
     <pageField fld="10" item="14" hier="-1"/>
-    <pageField fld="45" item="1" hier="-1"/>
   </pageFields>
-  <dataFields count="5">
-    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
-    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
-    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
-    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
-    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
   </dataFields>
-  <chartFormats count="21">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="21">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="9" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -49797,8 +49570,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000002000000}" name="PivotTable2" cacheId="46" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
-  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FEE7328-E767-497A-8049-35A88773E794}" name="PivotTable7" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="J41:J42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -49822,12 +49595,35 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item m="1" x="7"/>
+        <item x="1"/>
+        <item m="1" x="13"/>
+        <item m="1" x="15"/>
+        <item m="1" x="10"/>
+        <item m="1" x="6"/>
+        <item m="1" x="14"/>
+        <item m="1" x="12"/>
+        <item m="1" x="5"/>
+        <item m="1" x="16"/>
+        <item m="1" x="8"/>
+        <item m="1" x="18"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49865,44 +49661,19 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
     <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
+  <rowItems count="1">
+    <i/>
   </rowItems>
   <colItems count="1">
     <i/>
@@ -49910,41 +49681,159 @@
   <pageFields count="3">
     <pageField fld="32" item="9" hier="-1"/>
     <pageField fld="1" hier="-1"/>
-    <pageField fld="45" item="1" hier="-1"/>
+    <pageField fld="10" item="18" hier="-1"/>
   </pageFields>
-  <dataFields count="5">
-    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
-    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
-    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
-    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
-    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
   </dataFields>
-  <chartFormats count="15">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable10" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A54:B60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="35"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="1" item="2" hier="-1"/>
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="45" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="35" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="2" format="10" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -49953,110 +49842,11 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
+    <chartFormat chart="2" format="26">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
           </reference>
         </references>
       </pivotArea>
@@ -50074,171 +49864,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable1" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="AB5:AD10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item x="1"/>
-        <item m="1" x="11"/>
-        <item m="1" x="7"/>
-        <item m="1" x="13"/>
-        <item m="1" x="15"/>
-        <item m="1" x="10"/>
-        <item m="1" x="6"/>
-        <item m="1" x="14"/>
-        <item m="1" x="12"/>
-        <item m="1" x="5"/>
-        <item m="1" x="16"/>
-        <item m="1" x="8"/>
-        <item m="1" x="18"/>
-        <item x="2"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="11">
-        <item h="1" x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item h="1" x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item h="1" m="1" x="5"/>
-        <item h="1" m="1" x="7"/>
-        <item h="1" x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="10"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="45" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="2">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="10" baseItem="0"/>
-    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="10" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable1" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="AL10:AP17" firstHeaderRow="1" firstDataRow="3" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -50410,7 +50037,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D8B9FB5-5471-4500-848C-1623DA7CC3A0}" name="PivotTable4" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0D8B9FB5-5471-4500-848C-1623DA7CC3A0}" name="PivotTable4" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="G5:H8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField showAll="0"/>
@@ -50534,7 +50161,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable5" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0600-000000000000}" name="PivotTable5" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="B3:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -50640,7 +50267,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000000000000}" name="PivotTable1" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0800-000000000000}" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="11">
   <location ref="A6:B12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -50884,7 +50511,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0A00-000000000000}" name="PivotTable1" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0A00-000000000000}" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="B5:C13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -51161,7 +50788,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0C00-000000000000}" name="PivotTable2" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0C00-000000000000}" name="PivotTable2" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="D5:E13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -51486,7 +51113,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000000000000}" name="PivotTable1" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000000000000}" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="B9:C15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -51912,7 +51539,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000002000000}" name="PivotTable3" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0E00-000002000000}" name="PivotTable3" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="B29:H38" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -52309,7 +51936,1391 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000007000000}" name="PivotTable9" cacheId="46" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable3" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A40:A41" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="45" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000002000000}" name="PivotTable2" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="45" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
+    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
+    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
+    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
+    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  </dataFields>
+  <chartFormats count="15">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31FCE1EF-625E-43F6-9928-8FD8FD0AC1EA}" name="PivotTable11" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
+  <location ref="E51:F60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="3"/>
+        <item x="8"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="44"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="1" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Story Points" fld="13" baseField="44" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="18">
+    <chartFormat chart="2" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="2">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="3">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="4">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="5">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="6">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="7">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="16">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="17">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="3" format="18">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="44" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="AB5:AD10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" subtotalTop="0" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item x="1"/>
+        <item m="1" x="11"/>
+        <item m="1" x="7"/>
+        <item m="1" x="13"/>
+        <item m="1" x="15"/>
+        <item m="1" x="10"/>
+        <item m="1" x="6"/>
+        <item m="1" x="14"/>
+        <item m="1" x="12"/>
+        <item m="1" x="5"/>
+        <item m="1" x="16"/>
+        <item m="1" x="8"/>
+        <item m="1" x="18"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="11">
+        <item h="1" x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item h="1" x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item h="1" m="1" x="5"/>
+        <item h="1" m="1" x="7"/>
+        <item h="1" x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="10"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="45" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="2">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="10" baseItem="0"/>
+    <dataField name="Sum of Epic Remaining Estimate" fld="16" baseField="10" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000006000000}" name="PivotTable8" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="G41:G42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item m="1" x="7"/>
+        <item x="1"/>
+        <item m="1" x="13"/>
+        <item m="1" x="15"/>
+        <item m="1" x="10"/>
+        <item m="1" x="6"/>
+        <item m="1" x="14"/>
+        <item m="1" x="12"/>
+        <item m="1" x="5"/>
+        <item m="1" x="16"/>
+        <item m="1" x="8"/>
+        <item m="1" x="18"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="17" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000004000000}" name="PivotTable4" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
+  <location ref="D29:E34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item m="1" x="7"/>
+        <item x="1"/>
+        <item m="1" x="13"/>
+        <item m="1" x="15"/>
+        <item m="1" x="10"/>
+        <item m="1" x="6"/>
+        <item m="1" x="14"/>
+        <item m="1" x="12"/>
+        <item m="1" x="5"/>
+        <item m="1" x="16"/>
+        <item m="1" x="8"/>
+        <item m="1" x="18"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="4">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="14" hier="-1"/>
+    <pageField fld="45" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
+    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
+    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
+    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
+    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  </dataFields>
+  <chartFormats count="21">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="9" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000007000000}" name="PivotTable9" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
   <location ref="G29:H34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -52718,724 +53729,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FEE7328-E767-497A-8049-35A88773E794}" name="PivotTable7" cacheId="46" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="J41:J42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item m="1" x="7"/>
-        <item x="1"/>
-        <item m="1" x="13"/>
-        <item m="1" x="15"/>
-        <item m="1" x="10"/>
-        <item m="1" x="6"/>
-        <item m="1" x="14"/>
-        <item m="1" x="12"/>
-        <item m="1" x="5"/>
-        <item m="1" x="16"/>
-        <item m="1" x="8"/>
-        <item m="1" x="18"/>
-        <item x="2"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="18" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable3" cacheId="46" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A40:A41" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="45" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31FCE1EF-625E-43F6-9928-8FD8FD0AC1EA}" name="PivotTable11" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
-  <location ref="E51:F60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="10">
-        <item x="0"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="3"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="44"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="1" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Story Points" fld="13" baseField="44" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="18">
-    <chartFormat chart="2" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="3">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="4">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="5">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="6">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="7">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="5"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="16">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="17">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="7"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="3" format="18">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="44" count="1" selected="0">
-            <x v="8"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000006000000}" name="PivotTable8" cacheId="46" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="G41:G42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item m="1" x="7"/>
-        <item x="1"/>
-        <item m="1" x="13"/>
-        <item m="1" x="15"/>
-        <item m="1" x="10"/>
-        <item m="1" x="6"/>
-        <item m="1" x="14"/>
-        <item m="1" x="12"/>
-        <item m="1" x="5"/>
-        <item m="1" x="16"/>
-        <item m="1" x="8"/>
-        <item m="1" x="18"/>
-        <item x="2"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="17" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFE64A30-B41F-4AE4-94E0-976FA0DF52E6}" name="PivotTable6" cacheId="46" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFE64A30-B41F-4AE4-94E0-976FA0DF52E6}" name="PivotTable6" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
   <location ref="J29:K34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
@@ -53886,301 +54181,6 @@
       </pivotArea>
     </chartFormat>
   </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable10" cacheId="46" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A54:B60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="35"/>
-  </rowFields>
-  <rowItems count="6">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="1" item="2" hier="-1"/>
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="45" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="35" baseItem="0"/>
-  </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="2" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="2" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000005000000}" name="PivotTable5" cacheId="46" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="D41:D42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item m="1" x="7"/>
-        <item x="1"/>
-        <item m="1" x="13"/>
-        <item m="1" x="15"/>
-        <item m="1" x="10"/>
-        <item m="1" x="6"/>
-        <item m="1" x="14"/>
-        <item m="1" x="12"/>
-        <item m="1" x="5"/>
-        <item m="1" x="16"/>
-        <item m="1" x="8"/>
-        <item m="1" x="18"/>
-        <item x="2"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="14" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -60830,16 +60830,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.5546875" customWidth="1"/>
     <col min="13" max="13" width="14.109375" customWidth="1"/>
@@ -61017,14 +61017,14 @@
       </c>
       <c r="Q3" s="40">
         <f>$Q$25*(100%-K3)</f>
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="R3" s="42">
         <v>465</v>
       </c>
       <c r="S3" s="40">
         <f>$Q$26*(100%-K3)</f>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="T3" s="42">
         <v>136</v>
@@ -61094,14 +61094,14 @@
       </c>
       <c r="Q4" s="40">
         <f>$Q$25*(100%-K4)</f>
-        <v>406.8656716417911</v>
+        <v>458.80597014925377</v>
       </c>
       <c r="R4" s="42">
         <v>442.3</v>
       </c>
       <c r="S4" s="42">
         <f>$Q$26*(100%-K4)</f>
-        <v>173.13432835820896</v>
+        <v>225.07462686567166</v>
       </c>
       <c r="T4" s="42">
         <v>138.30000000000001</v>
@@ -61175,7 +61175,7 @@
       </c>
       <c r="Q5" s="40">
         <f t="shared" ref="Q5:Q9" si="1">$Q$25*(100%-K5)</f>
-        <v>336.71641791044777</v>
+        <v>379.70149253731347</v>
       </c>
       <c r="R5" s="42">
         <f>GETPIVOTDATA("Epic Remaining Estimate",$AB$4)</f>
@@ -61183,7 +61183,7 @@
       </c>
       <c r="S5" s="42">
         <f t="shared" ref="S5:S9" si="2">$Q$26*(100%-K5)</f>
-        <v>143.28358208955225</v>
+        <v>186.26865671641792</v>
       </c>
       <c r="T5" s="42">
         <f>GETPIVOTDATA("Epic Remaining Estimate",$AB$4,"ST:Components","Admin")</f>
@@ -61263,12 +61263,12 @@
       <c r="P6" s="76"/>
       <c r="Q6" s="40">
         <f t="shared" ref="Q6" si="5">$Q$25*(100%-K6)</f>
-        <v>266.56716417910451</v>
+        <v>300.59701492537317</v>
       </c>
       <c r="R6" s="42"/>
       <c r="S6" s="42">
         <f t="shared" ref="S6" si="6">$Q$26*(100%-K6)</f>
-        <v>113.43283582089553</v>
+        <v>147.46268656716421</v>
       </c>
       <c r="T6" s="42"/>
       <c r="U6" s="40">
@@ -61329,12 +61329,12 @@
       <c r="P7" s="76"/>
       <c r="Q7" s="40">
         <f t="shared" si="1"/>
-        <v>196.41791044776119</v>
+        <v>221.49253731343282</v>
       </c>
       <c r="R7" s="42"/>
       <c r="S7" s="42">
         <f t="shared" si="2"/>
-        <v>83.582089552238799</v>
+        <v>108.65671641791045</v>
       </c>
       <c r="T7" s="42"/>
       <c r="U7" s="40">
@@ -61390,12 +61390,12 @@
       <c r="P8" s="76"/>
       <c r="Q8" s="40">
         <f t="shared" si="1"/>
-        <v>133.28358208955225</v>
+        <v>150.29850746268659</v>
       </c>
       <c r="R8" s="42"/>
       <c r="S8" s="42">
         <f t="shared" si="2"/>
-        <v>56.716417910447767</v>
+        <v>73.731343283582106</v>
       </c>
       <c r="T8" s="42"/>
       <c r="U8" s="40">
@@ -61455,12 +61455,12 @@
       <c r="P9" s="76"/>
       <c r="Q9" s="42">
         <f t="shared" si="1"/>
-        <v>63.134328358208982</v>
+        <v>71.194029850746304</v>
       </c>
       <c r="R9" s="42"/>
       <c r="S9" s="42">
         <f t="shared" si="2"/>
-        <v>26.865671641791057</v>
+        <v>34.925373134328375</v>
       </c>
       <c r="T9" s="42"/>
       <c r="U9" s="42">
@@ -61873,7 +61873,7 @@
         <v>135</v>
       </c>
       <c r="Q25">
-        <v>470</v>
+        <v>530</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
@@ -61906,7 +61906,7 @@
         <v>255</v>
       </c>
       <c r="Q26">
-        <v>200</v>
+        <v>260</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.3">
@@ -62672,7 +62672,7 @@
       </c>
       <c r="E3" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="F3" s="40">
         <v>443.8</v>
@@ -62700,7 +62700,7 @@
       </c>
       <c r="M3" s="58">
         <f>_ReleaseData!$Q$26</f>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="N3" s="40">
         <v>124.8</v>
@@ -62795,7 +62795,7 @@
       </c>
       <c r="E4" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="F4" s="40">
         <v>525</v>
@@ -62823,7 +62823,7 @@
       </c>
       <c r="M4" s="58">
         <f>_ReleaseData!$Q$26</f>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="N4" s="40">
         <v>184</v>
@@ -62919,7 +62919,7 @@
       </c>
       <c r="E5" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="F5" s="40">
         <f>GETPIVOTDATA("Stories Estimate", $AL$8, "Type", "Epic")</f>
@@ -62951,7 +62951,7 @@
       </c>
       <c r="M5" s="58">
         <f>_ReleaseData!$Q$26</f>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="N5" s="40">
         <f>GETPIVOTDATA("Stories Estimate", $AL$8, "Type", "Epic", "ST:Components", "Admin")</f>
@@ -63055,7 +63055,7 @@
       <c r="D6" s="57"/>
       <c r="E6" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
@@ -63072,7 +63072,7 @@
       <c r="L6" s="59"/>
       <c r="M6" s="58">
         <f>_ReleaseData!$Q$26</f>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="N6" s="40"/>
       <c r="O6" s="40"/>
@@ -63134,7 +63134,7 @@
       <c r="D7" s="57"/>
       <c r="E7" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
@@ -63151,7 +63151,7 @@
       <c r="L7" s="59"/>
       <c r="M7" s="58">
         <f>_ReleaseData!$Q$26</f>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="N7" s="40"/>
       <c r="O7" s="40"/>
@@ -63219,7 +63219,7 @@
       <c r="D8" s="57"/>
       <c r="E8" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="40"/>
@@ -63236,7 +63236,7 @@
       <c r="L8" s="59"/>
       <c r="M8" s="58">
         <f>_ReleaseData!$Q$26</f>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="N8" s="40"/>
       <c r="O8" s="40"/>
@@ -63304,7 +63304,7 @@
       <c r="D9" s="57"/>
       <c r="E9" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="40"/>
@@ -63321,7 +63321,7 @@
       <c r="L9" s="59"/>
       <c r="M9" s="58">
         <f>_ReleaseData!$Q$26</f>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="N9" s="40"/>
       <c r="O9" s="40"/>
@@ -63383,7 +63383,7 @@
       <c r="D10" s="57"/>
       <c r="E10" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="F10" s="40"/>
       <c r="G10" s="40"/>
@@ -63400,7 +63400,7 @@
       <c r="L10" s="59"/>
       <c r="M10" s="58">
         <f>_ReleaseData!$Q$26</f>
-        <v>200</v>
+        <v>260</v>
       </c>
       <c r="N10" s="40"/>
       <c r="O10" s="40"/>

</xml_diff>

<commit_message>
Another Release scope adjustment from 530 to 630.
</commit_message>
<xml_diff>
--- a/blueprint-jira-better-excel/Wavelength-Dashboard.xlsx
+++ b/blueprint-jira-better-excel/Wavelength-Dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\etc\blueprint-jira-better-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4261542C-476A-4AD8-8BEA-F0ABC4D4A32D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F895748-B0AE-4CC8-9D51-AA6C828DA165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20813,25 +20813,25 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>530</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>458.80597014925377</c:v>
+                  <c:v>545.37313432835822</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>379.70149253731347</c:v>
+                  <c:v>451.34328358208961</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>300.59701492537317</c:v>
+                  <c:v>357.31343283582095</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>221.49253731343282</c:v>
+                  <c:v>263.28358208955223</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>150.29850746268659</c:v>
+                  <c:v>178.65671641791047</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>71.194029850746304</c:v>
+                  <c:v>84.626865671641823</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -21765,28 +21765,28 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>530</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>530</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>530</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>530</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>530</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>530</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>530</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>530</c:v>
+                  <c:v>630</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -43634,7 +43634,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43887.4569849537" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="109" xr:uid="{00000000-000A-0000-FFFF-FFFF0C000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Alex Folomechine" refreshedDate="43887.496244212962" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="109" xr:uid="{00000000-000A-0000-FFFF-FFFF0C000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="issues"/>
   </cacheSource>
@@ -49441,8 +49441,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000005000000}" name="PivotTable5" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="D41:D42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFE64A30-B41F-4AE4-94E0-976FA0DF52E6}" name="PivotTable6" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
+  <location ref="J29:K34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -49494,7 +49494,7 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49532,31 +49532,366 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
     <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowItems count="1">
-    <i/>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
-  <pageFields count="3">
+  <pageFields count="4">
     <pageField fld="32" item="9" hier="-1"/>
     <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="14" hier="-1"/>
+    <pageField fld="10" item="18" hier="-1"/>
+    <pageField fld="45" item="1" hier="-1"/>
   </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  <dataFields count="5">
+    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
+    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
+    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
+    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
+    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
   </dataFields>
+  <chartFormats count="33">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="18" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="18" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="18" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="18" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="18" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="18" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -49570,8 +49905,286 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FEE7328-E767-497A-8049-35A88773E794}" name="PivotTable7" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="J41:J42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000002000000}" name="PivotTable2" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
+  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="-2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+    <i i="3">
+      <x v="3"/>
+    </i>
+    <i i="4">
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="45" item="1" hier="-1"/>
+  </pageFields>
+  <dataFields count="5">
+    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
+    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
+    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
+    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
+    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
+  </dataFields>
+  <chartFormats count="15">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000007000000}" name="PivotTable9" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
+  <location ref="G29:H34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
@@ -49623,7 +50236,7 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
@@ -49661,179 +50274,87 @@
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="18" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable10" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
-  <location ref="A54:B60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="6"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="5"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="9">
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField subtotalTop="0" showAll="0"/>
     <pivotField showAll="0"/>
     <pivotField axis="axisPage" showAll="0">
       <items count="5">
         <item m="1" x="3"/>
-        <item x="0"/>
         <item x="2"/>
         <item x="1"/>
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="1">
-    <field x="35"/>
+    <field x="-2"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="5">
     <i>
+      <x/>
+    </i>
+    <i i="1">
       <x v="1"/>
     </i>
-    <i>
+    <i i="2">
       <x v="2"/>
     </i>
-    <i>
+    <i i="3">
       <x v="3"/>
     </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i t="grand">
-      <x/>
+    <i i="4">
+      <x v="4"/>
     </i>
   </rowItems>
   <colItems count="1">
     <i/>
   </colItems>
-  <pageFields count="3">
-    <pageField fld="1" item="2" hier="-1"/>
+  <pageFields count="4">
     <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="45" item="2" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="17" hier="-1"/>
+    <pageField fld="45" item="1" hier="-1"/>
   </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="35" baseItem="0"/>
+  <dataFields count="5">
+    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
+    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
+    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
+    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
+    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
   </dataFields>
-  <chartFormats count="2">
-    <chartFormat chart="2" format="10" series="1">
+  <chartFormats count="27">
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="1" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -49842,11 +50363,218 @@
         </references>
       </pivotArea>
     </chartFormat>
-    <chartFormat chart="2" format="26">
+    <chartFormat chart="0" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="11">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="13">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="14">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="15">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="22" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="25">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="4" format="27">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="8">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="9">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="10">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="11">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="7" format="12">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="19" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="20">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="21">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="22">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="23">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="14" format="24">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="4"/>
           </reference>
         </references>
       </pivotArea>
@@ -51936,398 +52664,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable3" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A40:A41" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowItems count="1">
-    <i/>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="45" item="2" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000002000000}" name="PivotTable2" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="9">
-  <location ref="A29:B34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="3">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="45" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="5">
-    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
-    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
-    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
-    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
-    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
-  </dataFields>
-  <chartFormats count="15">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{31FCE1EF-625E-43F6-9928-8FD8FD0AC1EA}" name="PivotTable11" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="4">
   <location ref="E51:F60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="49">
@@ -52671,7 +53007,136 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5FEE7328-E767-497A-8049-35A88773E794}" name="PivotTable7" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="J41:J42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item m="1" x="7"/>
+        <item x="1"/>
+        <item m="1" x="13"/>
+        <item m="1" x="15"/>
+        <item m="1" x="10"/>
+        <item m="1" x="6"/>
+        <item m="1" x="14"/>
+        <item m="1" x="12"/>
+        <item m="1" x="5"/>
+        <item m="1" x="16"/>
+        <item m="1" x="8"/>
+        <item m="1" x="18"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="18" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="PivotTable1" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="AB5:AD10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="49">
@@ -52834,6 +53299,172 @@
 </pivotTableDefinition>
 </file>
 
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000001000000}" name="PivotTable10" cacheId="30" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A54:B60" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="6"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField subtotalTop="0" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="35"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="1" item="2" hier="-1"/>
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="45" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="35" baseItem="0"/>
+  </dataFields>
+  <chartFormats count="2">
+    <chartFormat chart="2" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="26">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000006000000}" name="PivotTable8" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="G41:G42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
@@ -52964,6 +53595,249 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000005000000}" name="PivotTable5" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="D41:D42" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="20">
+        <item x="0"/>
+        <item m="1" x="11"/>
+        <item m="1" x="7"/>
+        <item x="1"/>
+        <item m="1" x="13"/>
+        <item m="1" x="15"/>
+        <item m="1" x="10"/>
+        <item m="1" x="6"/>
+        <item m="1" x="14"/>
+        <item m="1" x="12"/>
+        <item m="1" x="5"/>
+        <item m="1" x="16"/>
+        <item m="1" x="8"/>
+        <item m="1" x="18"/>
+        <item x="2"/>
+        <item m="1" x="17"/>
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="10" item="14" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000003000000}" name="PivotTable3" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A40:A41" firstHeaderRow="1" firstDataRow="1" firstDataCol="0" rowPageCount="3" colPageCount="1"/>
+  <pivotFields count="49">
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="9">
+        <item h="1" x="0"/>
+        <item h="1" x="6"/>
+        <item x="2"/>
+        <item h="1" x="4"/>
+        <item h="1" x="3"/>
+        <item h="1" x="5"/>
+        <item h="1" x="1"/>
+        <item h="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField dataField="1" subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
+      <items count="11">
+        <item x="0"/>
+        <item m="1" x="9"/>
+        <item m="1" x="8"/>
+        <item x="1"/>
+        <item m="1" x="4"/>
+        <item m="1" x="6"/>
+        <item m="1" x="5"/>
+        <item m="1" x="7"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField subtotalTop="0" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item m="1" x="3"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowItems count="1">
+    <i/>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="3">
+    <pageField fld="32" item="9" hier="-1"/>
+    <pageField fld="1" hier="-1"/>
+    <pageField fld="45" item="2" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Sum of Epic Total Estimate" fld="15" baseField="0" baseItem="514"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000004000000}" name="PivotTable4" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="14">
   <location ref="D29:E34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
   <pivotFields count="49">
@@ -53298,880 +54172,6 @@
       </pivotArea>
     </chartFormat>
     <chartFormat chart="9" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000007000000}" name="PivotTable9" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="17">
-  <location ref="G29:H34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item m="1" x="7"/>
-        <item x="1"/>
-        <item m="1" x="13"/>
-        <item m="1" x="15"/>
-        <item m="1" x="10"/>
-        <item m="1" x="6"/>
-        <item m="1" x="14"/>
-        <item m="1" x="12"/>
-        <item m="1" x="5"/>
-        <item m="1" x="16"/>
-        <item m="1" x="8"/>
-        <item m="1" x="18"/>
-        <item x="2"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="4">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="17" hier="-1"/>
-    <pageField fld="45" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="5">
-    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
-    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
-    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
-    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
-    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
-  </dataFields>
-  <chartFormats count="27">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="21">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{AFE64A30-B41F-4AE4-94E0-976FA0DF52E6}" name="PivotTable6" cacheId="30" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
-  <location ref="J29:K34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="4" colPageCount="1"/>
-  <pivotFields count="49">
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="9">
-        <item h="1" x="0"/>
-        <item h="1" x="6"/>
-        <item x="2"/>
-        <item h="1" x="4"/>
-        <item h="1" x="3"/>
-        <item h="1" x="5"/>
-        <item h="1" x="1"/>
-        <item h="1" x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="20">
-        <item x="0"/>
-        <item m="1" x="11"/>
-        <item m="1" x="7"/>
-        <item x="1"/>
-        <item m="1" x="13"/>
-        <item m="1" x="15"/>
-        <item m="1" x="10"/>
-        <item m="1" x="6"/>
-        <item m="1" x="14"/>
-        <item m="1" x="12"/>
-        <item m="1" x="5"/>
-        <item m="1" x="16"/>
-        <item m="1" x="8"/>
-        <item m="1" x="18"/>
-        <item x="2"/>
-        <item m="1" x="17"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField axis="axisPage" subtotalTop="0" showAll="0">
-      <items count="11">
-        <item x="0"/>
-        <item m="1" x="9"/>
-        <item m="1" x="8"/>
-        <item x="1"/>
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="5"/>
-        <item m="1" x="7"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField subtotalTop="0" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item m="1" x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="-2"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-    <i i="3">
-      <x v="3"/>
-    </i>
-    <i i="4">
-      <x v="4"/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <pageFields count="4">
-    <pageField fld="32" item="9" hier="-1"/>
-    <pageField fld="1" hier="-1"/>
-    <pageField fld="10" item="18" hier="-1"/>
-    <pageField fld="45" item="1" hier="-1"/>
-  </pageFields>
-  <dataFields count="5">
-    <dataField name="Done" fld="47" baseField="0" baseItem="32"/>
-    <dataField name="In Validation" fld="41" baseField="0" baseItem="32"/>
-    <dataField name="In Dev" fld="40" baseField="0" baseItem="32"/>
-    <dataField name="Ready" fld="39" baseField="0" baseItem="32"/>
-    <dataField name="Not Decomposed" fld="48" baseField="0" baseItem="32"/>
-  </dataFields>
-  <chartFormats count="33">
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="10" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="13">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="14">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="15">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="22" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="25">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="26">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="4" format="27">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="7" format="12">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="19" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="20">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="21">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="22">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="23">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="14" format="24">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="18" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="18" format="8">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="18" format="9">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="18" format="10">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="18" format="11">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="18" format="12">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -60826,12 +60826,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AD66"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
@@ -61017,7 +61019,7 @@
       </c>
       <c r="Q3" s="40">
         <f>$Q$25*(100%-K3)</f>
-        <v>530</v>
+        <v>630</v>
       </c>
       <c r="R3" s="42">
         <v>465</v>
@@ -61094,7 +61096,7 @@
       </c>
       <c r="Q4" s="40">
         <f>$Q$25*(100%-K4)</f>
-        <v>458.80597014925377</v>
+        <v>545.37313432835822</v>
       </c>
       <c r="R4" s="42">
         <v>442.3</v>
@@ -61175,7 +61177,7 @@
       </c>
       <c r="Q5" s="40">
         <f t="shared" ref="Q5:Q9" si="1">$Q$25*(100%-K5)</f>
-        <v>379.70149253731347</v>
+        <v>451.34328358208961</v>
       </c>
       <c r="R5" s="42">
         <f>GETPIVOTDATA("Epic Remaining Estimate",$AB$4)</f>
@@ -61263,7 +61265,7 @@
       <c r="P6" s="76"/>
       <c r="Q6" s="40">
         <f t="shared" ref="Q6" si="5">$Q$25*(100%-K6)</f>
-        <v>300.59701492537317</v>
+        <v>357.31343283582095</v>
       </c>
       <c r="R6" s="42"/>
       <c r="S6" s="42">
@@ -61329,7 +61331,7 @@
       <c r="P7" s="76"/>
       <c r="Q7" s="40">
         <f t="shared" si="1"/>
-        <v>221.49253731343282</v>
+        <v>263.28358208955223</v>
       </c>
       <c r="R7" s="42"/>
       <c r="S7" s="42">
@@ -61390,7 +61392,7 @@
       <c r="P8" s="76"/>
       <c r="Q8" s="40">
         <f t="shared" si="1"/>
-        <v>150.29850746268659</v>
+        <v>178.65671641791047</v>
       </c>
       <c r="R8" s="42"/>
       <c r="S8" s="42">
@@ -61455,7 +61457,7 @@
       <c r="P9" s="76"/>
       <c r="Q9" s="42">
         <f t="shared" si="1"/>
-        <v>71.194029850746304</v>
+        <v>84.626865671641823</v>
       </c>
       <c r="R9" s="42"/>
       <c r="S9" s="42">
@@ -61873,7 +61875,7 @@
         <v>135</v>
       </c>
       <c r="Q25">
-        <v>530</v>
+        <v>630</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.3">
@@ -62672,7 +62674,7 @@
       </c>
       <c r="E3" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>530</v>
+        <v>630</v>
       </c>
       <c r="F3" s="40">
         <v>443.8</v>
@@ -62795,7 +62797,7 @@
       </c>
       <c r="E4" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>530</v>
+        <v>630</v>
       </c>
       <c r="F4" s="40">
         <v>525</v>
@@ -62919,7 +62921,7 @@
       </c>
       <c r="E5" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>530</v>
+        <v>630</v>
       </c>
       <c r="F5" s="40">
         <f>GETPIVOTDATA("Stories Estimate", $AL$8, "Type", "Epic")</f>
@@ -63055,7 +63057,7 @@
       <c r="D6" s="57"/>
       <c r="E6" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>530</v>
+        <v>630</v>
       </c>
       <c r="F6" s="40"/>
       <c r="G6" s="40"/>
@@ -63134,7 +63136,7 @@
       <c r="D7" s="57"/>
       <c r="E7" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>530</v>
+        <v>630</v>
       </c>
       <c r="F7" s="40"/>
       <c r="G7" s="40"/>
@@ -63219,7 +63221,7 @@
       <c r="D8" s="57"/>
       <c r="E8" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>530</v>
+        <v>630</v>
       </c>
       <c r="F8" s="40"/>
       <c r="G8" s="40"/>
@@ -63304,7 +63306,7 @@
       <c r="D9" s="57"/>
       <c r="E9" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>530</v>
+        <v>630</v>
       </c>
       <c r="F9" s="40"/>
       <c r="G9" s="40"/>
@@ -63383,7 +63385,7 @@
       <c r="D10" s="57"/>
       <c r="E10" s="58">
         <f>_ReleaseData!$Q$25</f>
-        <v>530</v>
+        <v>630</v>
       </c>
       <c r="F10" s="40"/>
       <c r="G10" s="40"/>

</xml_diff>